<commit_message>
Fix loi lam bai
</commit_message>
<xml_diff>
--- a/TestingOnline/uploads/Câu hỏi.xlsx
+++ b/TestingOnline/uploads/Câu hỏi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thong\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AAD3DF-0A2C-4B4F-8988-31C1122058D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF415A9D-B8A9-42A1-AF9D-447E8471E486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="2070" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2070" yWindow="2070" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiếng Anh" sheetId="2" r:id="rId1"/>
@@ -1035,17 +1035,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1266,7 +1266,9 @@
   </sheetPr>
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1275,946 +1277,950 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="10">
+      <c r="A13" s="11">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="10">
+      <c r="A16" s="11">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="10">
+      <c r="A17" s="11">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="10">
+      <c r="A18" s="11">
         <v>17</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
+      <c r="A20" s="11">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="10">
+      <c r="A21" s="11">
         <v>20</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="13">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="13">
+      <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
+      <c r="A24" s="9">
         <v>23</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="13">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="13">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="13">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="13">
+      <c r="A28" s="9">
         <v>27</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="13">
+      <c r="A29" s="9">
         <v>28</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="13">
+      <c r="A30" s="9">
         <v>29</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="13">
+      <c r="A31" s="9">
         <v>30</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="13">
+      <c r="A32" s="9">
         <v>31</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="13">
+      <c r="A33" s="9">
         <v>32</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="13">
+      <c r="A34" s="9">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="12" t="s">
         <v>261</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="13">
+      <c r="A35" s="9">
         <v>34</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="13">
+      <c r="A36" s="9">
         <v>35</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="13">
+      <c r="A37" s="9">
         <v>36</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G37" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="13">
+      <c r="A38" s="9">
         <v>37</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="G38" s="10" t="s">
+      <c r="G38" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="13">
+      <c r="A39" s="9">
         <v>38</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="12" t="s">
         <v>286</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="G39" s="10" t="s">
+      <c r="G39" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="11" t="s">
+      <c r="A40" s="9">
+        <v>39</v>
+      </c>
+      <c r="B40" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F40" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="G40" s="10" t="s">
+      <c r="G40" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="12" t="s">
+      <c r="A41" s="9">
+        <v>40</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G41" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
+      <c r="A42" s="7"/>
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
@@ -6061,8 +6067,8 @@
   </sheetPr>
   <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6559,10 +6565,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
-        <v>21</v>
-      </c>
+    <row r="22" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>